<commit_message>
Minor changes to specifications
</commit_message>
<xml_diff>
--- a/WinningsDistribution.xlsx
+++ b/WinningsDistribution.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Java\BlackjackAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="25200" windowHeight="12120" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="25200" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alg" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Under Thresh</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Red areas indicate that the shuffle gave better results than without</t>
+  </si>
+  <si>
+    <t>Best Wins</t>
   </si>
 </sst>
 </file>
@@ -109,35 +112,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -442,11 +417,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="293754568"/>
-        <c:axId val="293754960"/>
+        <c:axId val="371223440"/>
+        <c:axId val="371221088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="293754568"/>
+        <c:axId val="371223440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293754960"/>
+        <c:crossAx val="371221088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -552,7 +527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293754960"/>
+        <c:axId val="371221088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293754568"/>
+        <c:crossAx val="371223440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -916,11 +891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="293413400"/>
-        <c:axId val="293413792"/>
+        <c:axId val="371221872"/>
+        <c:axId val="371223832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="293413400"/>
+        <c:axId val="371221872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293413792"/>
+        <c:crossAx val="371223832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1026,7 +1001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293413792"/>
+        <c:axId val="371223832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293413400"/>
+        <c:crossAx val="371221872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2566,16 +2541,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T22"/>
+  <dimension ref="A2:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="18" width="9.140625" style="1"/>
     <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -2596,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="1">
-        <f>B2/C2</f>
+        <f t="shared" ref="T2:T21" si="0">B2/C2</f>
         <v>0.53555579441979029</v>
       </c>
     </row>
@@ -2615,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="T3" s="1">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>0.53562653562653562</v>
       </c>
     </row>
@@ -2630,11 +2606,11 @@
         <v>0.65129999999999999</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" ref="S4:S21" si="0">S3+1</f>
+        <f t="shared" ref="S4:S21" si="1">S3+1</f>
         <v>3</v>
       </c>
       <c r="T4" s="1">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>0.53539075694764315</v>
       </c>
     </row>
@@ -2649,11 +2625,11 @@
         <v>0.65129000000000004</v>
       </c>
       <c r="S5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="T5" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="T5" s="1">
-        <f>B5/C5</f>
         <v>0.53541433155737073</v>
       </c>
     </row>
@@ -2668,11 +2644,11 @@
         <v>0.65151000000000003</v>
       </c>
       <c r="S6" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T6" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="T6" s="1">
-        <f>B6/C6</f>
         <v>0.53489585731608114</v>
       </c>
     </row>
@@ -2687,11 +2663,11 @@
         <v>0.65064999999999995</v>
       </c>
       <c r="S7" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="T7" s="1">
-        <f>B7/C7</f>
         <v>0.53692461384769086</v>
       </c>
     </row>
@@ -2706,11 +2682,11 @@
         <v>0.64932999999999996</v>
       </c>
       <c r="S8" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T8" s="1">
-        <f>B8/C8</f>
         <v>0.54004897355735915</v>
       </c>
     </row>
@@ -2725,11 +2701,11 @@
         <v>0.64695999999999998</v>
       </c>
       <c r="S9" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="T9" s="1">
-        <f>B9/C9</f>
         <v>0.54569061456658841</v>
       </c>
     </row>
@@ -2744,11 +2720,11 @@
         <v>0.64149</v>
       </c>
       <c r="S10" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="T10" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="T10" s="1">
-        <f>B10/C10</f>
         <v>0.55887075402578368</v>
       </c>
     </row>
@@ -2763,11 +2739,11 @@
         <v>0.63197000000000003</v>
       </c>
       <c r="S11" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="T11" s="1">
-        <f>B11/C11</f>
         <v>0.58235359273383236</v>
       </c>
     </row>
@@ -2782,11 +2758,11 @@
         <v>0.61621000000000004</v>
       </c>
       <c r="S12" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="T12" s="1">
-        <f>B12/C12</f>
         <v>0.62282338813066973</v>
       </c>
     </row>
@@ -2801,11 +2777,11 @@
         <v>0.59497999999999995</v>
       </c>
       <c r="S13" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="T13" s="1">
-        <f>B13/C13</f>
         <v>0.68072876399206705</v>
       </c>
     </row>
@@ -2820,11 +2796,11 @@
         <v>0.57071000000000005</v>
       </c>
       <c r="S14" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="T14" s="1">
-        <f>B14/C14</f>
         <v>0.74447617879483441</v>
       </c>
     </row>
@@ -2839,11 +2815,11 @@
         <v>0.54888000000000003</v>
       </c>
       <c r="S15" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="T15" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="T15" s="1">
-        <f>B15/C15</f>
         <v>0.8023429529223145</v>
       </c>
     </row>
@@ -2858,11 +2834,11 @@
         <v>0.53049000000000002</v>
       </c>
       <c r="S16" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="T16" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="T16" s="1">
-        <f>B16/C16</f>
         <v>0.84896982035476631</v>
       </c>
     </row>
@@ -2877,11 +2853,11 @@
         <v>0.51429000000000002</v>
       </c>
       <c r="S17" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="T17" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="T17" s="1">
-        <f>B17/C17</f>
         <v>0.88590095082540976</v>
       </c>
     </row>
@@ -2896,11 +2872,11 @@
         <v>0.50166999999999995</v>
       </c>
       <c r="S18" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="T18" s="1">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="T18" s="1">
-        <f>B18/C18</f>
         <v>0.90577471246038244</v>
       </c>
     </row>
@@ -2915,11 +2891,11 @@
         <v>0.49703999999999998</v>
       </c>
       <c r="S19" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="T19" s="1">
-        <f>B19/C19</f>
         <v>0.88990825688073394</v>
       </c>
     </row>
@@ -2934,11 +2910,11 @@
         <v>0.51966000000000001</v>
       </c>
       <c r="S20" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="T20" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="T20" s="1">
-        <f>B20/C20</f>
         <v>0.76748258476696307</v>
       </c>
     </row>
@@ -2953,29 +2929,30 @@
         <v>0.57525000000000004</v>
       </c>
       <c r="S21" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="T21" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="T21" s="1">
-        <f>B21/C21</f>
         <v>0.55289004780530204</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <f>MAX(B2:B21)</f>
-        <v>0.45561000000000001</v>
-      </c>
-      <c r="C22" s="1">
-        <f>MIN(C2:C21)</f>
-        <v>0.49703999999999998</v>
-      </c>
       <c r="S22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T22" s="1">
         <f>MAX(T2:T21)</f>
         <v>0.90577471246038244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
+        <f>MAX(B2:B21)</f>
+        <v>0.45561000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7617,7 +7594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -11262,59 +11239,59 @@
         <v>0.1</v>
       </c>
       <c r="G37" s="1">
-        <f>C1/D1</f>
+        <f t="shared" ref="G37:G50" si="32">C1/D1</f>
         <v>0.78555740076070069</v>
       </c>
       <c r="H37" s="1">
-        <f>G1/H1</f>
+        <f t="shared" ref="H37:H50" si="33">G1/H1</f>
         <v>0.78491744756804993</v>
       </c>
       <c r="I37" s="1">
-        <f>K1/L1</f>
+        <f t="shared" ref="I37:I50" si="34">K1/L1</f>
         <v>0.78501303059512328</v>
       </c>
       <c r="J37" s="1">
-        <f>O1/P1</f>
+        <f t="shared" ref="J37:J50" si="35">O1/P1</f>
         <v>0.78456706403026621</v>
       </c>
       <c r="K37" s="1">
-        <f>S1/T1</f>
+        <f t="shared" ref="K37:K50" si="36">S1/T1</f>
         <v>0.78472631222002109</v>
       </c>
       <c r="L37" s="1">
-        <f>W1/X1</f>
+        <f t="shared" ref="L37:L50" si="37">W1/X1</f>
         <v>0.78542734203431597</v>
       </c>
       <c r="M37" s="1">
-        <f>AA1/AB1</f>
+        <f t="shared" ref="M37:M50" si="38">AA1/AB1</f>
         <v>0.78466260953366773</v>
       </c>
       <c r="N37" s="1">
-        <f>AE1/AF1</f>
+        <f t="shared" ref="N37:N50" si="39">AE1/AF1</f>
         <v>0.78526796872210514</v>
       </c>
       <c r="O37" s="1">
-        <f>AI1/AJ1</f>
+        <f t="shared" ref="O37:O50" si="40">AI1/AJ1</f>
         <v>0.78456706403026621</v>
       </c>
       <c r="P37" s="1">
-        <f>AM1/AN1</f>
+        <f t="shared" ref="P37:P50" si="41">AM1/AN1</f>
         <v>0.78463075989577757</v>
       </c>
       <c r="Q37" s="1">
-        <f>AQ1/AR1</f>
+        <f t="shared" ref="Q37:Q50" si="42">AQ1/AR1</f>
         <v>0.78469446030839518</v>
       </c>
       <c r="R37" s="1">
-        <f>AU1/AV1</f>
+        <f t="shared" ref="R37:R50" si="43">AU1/AV1</f>
         <v>0.78491744756804993</v>
       </c>
       <c r="S37" s="1">
-        <f>AY1/AZ1</f>
+        <f t="shared" ref="S37:S50" si="44">AY1/AZ1</f>
         <v>0.78510862385976188</v>
       </c>
       <c r="T37" s="1">
-        <f>BC1/BD1</f>
+        <f t="shared" ref="T37:T50" si="45">BC1/BD1</f>
         <v>0.78424865289226708</v>
       </c>
     </row>
@@ -11324,741 +11301,741 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="G38" s="1">
-        <f>C2/D2</f>
+        <f t="shared" si="32"/>
         <v>0.78848871951764976</v>
       </c>
       <c r="H38" s="1">
-        <f>G2/H2</f>
+        <f t="shared" si="33"/>
         <v>0.78783977110157366</v>
       </c>
       <c r="I38" s="1">
-        <f>K2/L2</f>
+        <f t="shared" si="34"/>
         <v>0.78808148373365761</v>
       </c>
       <c r="J38" s="1">
-        <f>O2/P2</f>
+        <f t="shared" si="35"/>
         <v>0.78669073104483478</v>
       </c>
       <c r="K38" s="1">
-        <f>S2/T2</f>
+        <f t="shared" si="36"/>
         <v>0.78451737245034525</v>
       </c>
       <c r="L38" s="1">
-        <f>W2/X2</f>
+        <f t="shared" si="37"/>
         <v>0.78494930743966873</v>
       </c>
       <c r="M38" s="1">
-        <f>AA2/AB2</f>
+        <f t="shared" si="38"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="N38" s="1">
-        <f>AE2/AF2</f>
+        <f t="shared" si="39"/>
         <v>0.78501303059512328</v>
       </c>
       <c r="O38" s="1">
-        <f>AI2/AJ2</f>
+        <f t="shared" si="40"/>
         <v>0.78501303059512328</v>
       </c>
       <c r="P38" s="1">
-        <f>AM2/AN2</f>
+        <f t="shared" si="41"/>
         <v>0.78431232602954815</v>
       </c>
       <c r="Q38" s="1">
-        <f>AQ2/AR2</f>
+        <f t="shared" si="42"/>
         <v>0.78504489387908105</v>
       </c>
       <c r="R38" s="1">
-        <f>AU2/AV2</f>
+        <f t="shared" si="43"/>
         <v>0.78510862385976188</v>
       </c>
       <c r="S38" s="1">
-        <f>AY2/AZ2</f>
+        <f t="shared" si="44"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="T38" s="1">
-        <f>BC2/BD2</f>
+        <f t="shared" si="45"/>
         <v>0.78431232602954815</v>
       </c>
     </row>
     <row r="39" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F39" s="1">
-        <f t="shared" ref="F39:F50" si="32">F38+0.05</f>
+        <f t="shared" ref="F39:F50" si="46">F38+0.05</f>
         <v>0.2</v>
       </c>
       <c r="G39" s="1">
-        <f>C3/D3</f>
+        <f t="shared" si="32"/>
         <v>0.79005247792524136</v>
       </c>
       <c r="H39" s="1">
-        <f>G3/H3</f>
+        <f t="shared" si="33"/>
         <v>0.78903942870438315</v>
       </c>
       <c r="I39" s="1">
-        <f>K3/L3</f>
+        <f t="shared" si="34"/>
         <v>0.78866283751140698</v>
       </c>
       <c r="J39" s="1">
-        <f>O3/P3</f>
+        <f t="shared" si="35"/>
         <v>0.78761979688170503</v>
       </c>
       <c r="K39" s="1">
-        <f>S3/T3</f>
+        <f t="shared" si="36"/>
         <v>0.78513665494403484</v>
       </c>
       <c r="L39" s="1">
-        <f>W3/X3</f>
+        <f t="shared" si="37"/>
         <v>0.78485373123672508</v>
       </c>
       <c r="M39" s="1">
-        <f>AA3/AB3</f>
+        <f t="shared" si="38"/>
         <v>0.78504489387908105</v>
       </c>
       <c r="N39" s="1">
-        <f>AE3/AF3</f>
+        <f t="shared" si="39"/>
         <v>0.78504489387908105</v>
       </c>
       <c r="O39" s="1">
-        <f>AI3/AJ3</f>
+        <f t="shared" si="40"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="P39" s="1">
-        <f>AM3/AN3</f>
+        <f t="shared" si="41"/>
         <v>0.78469446030839518</v>
       </c>
       <c r="Q39" s="1">
-        <f>AQ3/AR3</f>
+        <f t="shared" si="42"/>
         <v>0.78504489387908105</v>
       </c>
       <c r="R39" s="1">
-        <f>AU3/AV3</f>
+        <f t="shared" si="43"/>
         <v>0.78488558883375581</v>
       </c>
       <c r="S39" s="1">
-        <f>AY3/AZ3</f>
+        <f t="shared" si="44"/>
         <v>0.78485373123672508</v>
       </c>
       <c r="T39" s="1">
-        <f>BC3/BD3</f>
+        <f t="shared" si="45"/>
         <v>0.78523609747389089</v>
       </c>
     </row>
     <row r="40" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F40" s="1">
+        <f t="shared" si="46"/>
+        <v>0.25</v>
+      </c>
+      <c r="G40" s="1">
         <f t="shared" si="32"/>
-        <v>0.25</v>
-      </c>
-      <c r="G40" s="1">
-        <f>C4/D4</f>
         <v>0.79234923653849609</v>
       </c>
       <c r="H40" s="1">
-        <f>G4/H4</f>
+        <f t="shared" si="33"/>
         <v>0.79127971601706759</v>
       </c>
       <c r="I40" s="1">
-        <f>K4/L4</f>
+        <f t="shared" si="34"/>
         <v>0.79073934702361759</v>
       </c>
       <c r="J40" s="1">
-        <f>O4/P4</f>
+        <f t="shared" si="35"/>
         <v>0.78905355097365404</v>
       </c>
       <c r="K40" s="1">
-        <f>S4/T4</f>
+        <f t="shared" si="36"/>
         <v>0.78656564393059447</v>
       </c>
       <c r="L40" s="1">
-        <f>W4/X4</f>
+        <f t="shared" si="37"/>
         <v>0.7864736889127133</v>
       </c>
       <c r="M40" s="1">
-        <f>AA4/AB4</f>
+        <f t="shared" si="38"/>
         <v>0.78656945784639576</v>
       </c>
       <c r="N40" s="1">
-        <f>AE4/AF4</f>
+        <f t="shared" si="39"/>
         <v>0.78633196355190282</v>
       </c>
       <c r="O40" s="1">
-        <f>AI4/AJ4</f>
+        <f t="shared" si="40"/>
         <v>0.78518254039096669</v>
       </c>
       <c r="P40" s="1">
-        <f>AM4/AN4</f>
+        <f t="shared" si="41"/>
         <v>0.78494930743966873</v>
       </c>
       <c r="Q40" s="1">
-        <f>AQ4/AR4</f>
+        <f t="shared" si="42"/>
         <v>0.78469446030839518</v>
       </c>
       <c r="R40" s="1">
-        <f>AU4/AV4</f>
+        <f t="shared" si="43"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="S40" s="1">
-        <f>AY4/AZ4</f>
+        <f t="shared" si="44"/>
         <v>0.78514049055660673</v>
       </c>
       <c r="T40" s="1">
-        <f>BC4/BD4</f>
+        <f t="shared" si="45"/>
         <v>0.78498116844867283</v>
       </c>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F41" s="1">
+        <f t="shared" si="46"/>
+        <v>0.3</v>
+      </c>
+      <c r="G41" s="1">
         <f t="shared" si="32"/>
-        <v>0.3</v>
-      </c>
-      <c r="G41" s="1">
-        <f>C5/D5</f>
         <v>0.83382176757902504</v>
       </c>
       <c r="H41" s="1">
-        <f>G5/H5</f>
+        <f t="shared" si="33"/>
         <v>0.83304482339508679</v>
       </c>
       <c r="I41" s="1">
-        <f>K5/L5</f>
+        <f t="shared" si="34"/>
         <v>0.8319105092728879</v>
       </c>
       <c r="J41" s="1">
-        <f>O5/P5</f>
+        <f t="shared" si="35"/>
         <v>0.83033466267252309</v>
       </c>
       <c r="K41" s="1">
-        <f>S5/T5</f>
+        <f t="shared" si="36"/>
         <v>0.82739896905325339</v>
       </c>
       <c r="L41" s="1">
-        <f>W5/X5</f>
+        <f t="shared" si="37"/>
         <v>0.82742047914297256</v>
       </c>
       <c r="M41" s="1">
-        <f>AA5/AB5</f>
+        <f t="shared" si="38"/>
         <v>0.8274053012932221</v>
       </c>
       <c r="N41" s="1">
-        <f>AE5/AF5</f>
+        <f t="shared" si="39"/>
         <v>0.82592443288012607</v>
       </c>
       <c r="O41" s="1">
-        <f>AI5/AJ5</f>
+        <f t="shared" si="40"/>
         <v>0.81284063658164374</v>
       </c>
       <c r="P41" s="1">
-        <f>AM5/AN5</f>
+        <f t="shared" si="41"/>
         <v>0.79676653598532532</v>
       </c>
       <c r="Q41" s="1">
-        <f>AQ5/AR5</f>
+        <f t="shared" si="42"/>
         <v>0.7854375345938901</v>
       </c>
       <c r="R41" s="1">
-        <f>AU5/AV5</f>
+        <f t="shared" si="43"/>
         <v>0.7852042273636104</v>
       </c>
       <c r="S41" s="1">
-        <f>AY5/AZ5</f>
+        <f t="shared" si="44"/>
         <v>0.78479001945421123</v>
       </c>
       <c r="T41" s="1">
-        <f>BC5/BD5</f>
+        <f t="shared" si="45"/>
         <v>0.78485373123672508</v>
       </c>
     </row>
     <row r="42" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F42" s="1">
+        <f t="shared" si="46"/>
+        <v>0.35</v>
+      </c>
+      <c r="G42" s="1">
         <f t="shared" si="32"/>
-        <v>0.35</v>
-      </c>
-      <c r="G42" s="1">
-        <f>C6/D6</f>
         <v>0.86527306967984929</v>
       </c>
       <c r="H42" s="1">
-        <f>G6/H6</f>
+        <f t="shared" si="33"/>
         <v>0.86452571772585318</v>
       </c>
       <c r="I42" s="1">
-        <f>K6/L6</f>
+        <f t="shared" si="34"/>
         <v>0.86317253302764363</v>
       </c>
       <c r="J42" s="1">
-        <f>O6/P6</f>
+        <f t="shared" si="35"/>
         <v>0.86050874165228486</v>
       </c>
       <c r="K42" s="1">
-        <f>S6/T6</f>
+        <f t="shared" si="36"/>
         <v>0.85809811009758563</v>
       </c>
       <c r="L42" s="1">
-        <f>W6/X6</f>
+        <f t="shared" si="37"/>
         <v>0.8577314181913519</v>
       </c>
       <c r="M42" s="1">
-        <f>AA6/AB6</f>
+        <f t="shared" si="38"/>
         <v>0.85467929675092957</v>
       </c>
       <c r="N42" s="1">
-        <f>AE6/AF6</f>
+        <f t="shared" si="39"/>
         <v>0.84081700616084798</v>
       </c>
       <c r="O42" s="1">
-        <f>AI6/AJ6</f>
+        <f t="shared" si="40"/>
         <v>0.82188076663073473</v>
       </c>
       <c r="P42" s="1">
-        <f>AM6/AN6</f>
+        <f t="shared" si="41"/>
         <v>0.80467394447657603</v>
       </c>
       <c r="Q42" s="1">
-        <f>AQ6/AR6</f>
+        <f t="shared" si="42"/>
         <v>0.78853206905805528</v>
       </c>
       <c r="R42" s="1">
-        <f>AU6/AV6</f>
+        <f t="shared" si="43"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="S42" s="1">
-        <f>AY6/AZ6</f>
+        <f t="shared" si="44"/>
         <v>0.78469446030839518</v>
       </c>
       <c r="T42" s="1">
-        <f>BC6/BD6</f>
+        <f t="shared" si="45"/>
         <v>0.78491744756804993</v>
       </c>
     </row>
     <row r="43" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F43" s="1">
+        <f t="shared" si="46"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G43" s="1">
         <f t="shared" si="32"/>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="G43" s="1">
-        <f>C7/D7</f>
         <v>0.89746950103108669</v>
       </c>
       <c r="H43" s="1">
-        <f>G7/H7</f>
+        <f t="shared" si="33"/>
         <v>0.89547500865750884</v>
       </c>
       <c r="I43" s="1">
-        <f>K7/L7</f>
+        <f t="shared" si="34"/>
         <v>0.89373679154658991</v>
       </c>
       <c r="J43" s="1">
-        <f>O7/P7</f>
+        <f t="shared" si="35"/>
         <v>0.89147405773472721</v>
       </c>
       <c r="K43" s="1">
-        <f>S7/T7</f>
+        <f t="shared" si="36"/>
         <v>0.8889612379347327</v>
       </c>
       <c r="L43" s="1">
-        <f>W7/X7</f>
+        <f t="shared" si="37"/>
         <v>0.88450091575091583</v>
       </c>
       <c r="M43" s="1">
-        <f>AA7/AB7</f>
+        <f t="shared" si="38"/>
         <v>0.87562999734737956</v>
       </c>
       <c r="N43" s="1">
-        <f>AE7/AF7</f>
+        <f t="shared" si="39"/>
         <v>0.85905336305231417</v>
       </c>
       <c r="O43" s="1">
-        <f>AI7/AJ7</f>
+        <f t="shared" si="40"/>
         <v>0.83204547963351361</v>
       </c>
       <c r="P43" s="1">
-        <f>AM7/AN7</f>
+        <f t="shared" si="41"/>
         <v>0.80472110761667215</v>
       </c>
       <c r="Q43" s="1">
-        <f>AQ7/AR7</f>
+        <f t="shared" si="42"/>
         <v>0.78925420149267089</v>
       </c>
       <c r="R43" s="1">
-        <f>AU7/AV7</f>
+        <f t="shared" si="43"/>
         <v>0.78488558883375581</v>
       </c>
       <c r="S43" s="1">
-        <f>AY7/AZ7</f>
+        <f t="shared" si="44"/>
         <v>0.78488558883375581</v>
       </c>
       <c r="T43" s="1">
-        <f>BC7/BD7</f>
+        <f t="shared" si="45"/>
         <v>0.78485373123672508</v>
       </c>
     </row>
     <row r="44" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F44" s="1">
+        <f t="shared" si="46"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G44" s="1">
         <f t="shared" si="32"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G44" s="1">
-        <f>C8/D8</f>
         <v>0.91928929027191519</v>
       </c>
       <c r="H44" s="1">
-        <f>G8/H8</f>
+        <f t="shared" si="33"/>
         <v>0.91806846253381968</v>
       </c>
       <c r="I44" s="1">
-        <f>K8/L8</f>
+        <f t="shared" si="34"/>
         <v>0.91627843244724583</v>
       </c>
       <c r="J44" s="1">
-        <f>O8/P8</f>
+        <f t="shared" si="35"/>
         <v>0.91341720715792762</v>
       </c>
       <c r="K44" s="1">
-        <f>S8/T8</f>
+        <f t="shared" si="36"/>
         <v>0.90785049272094698</v>
       </c>
       <c r="L44" s="1">
-        <f>W8/X8</f>
+        <f t="shared" si="37"/>
         <v>0.9007862151563738</v>
       </c>
       <c r="M44" s="1">
-        <f>AA8/AB8</f>
+        <f t="shared" si="38"/>
         <v>0.88584631836235861</v>
       </c>
       <c r="N44" s="1">
-        <f>AE8/AF8</f>
+        <f t="shared" si="39"/>
         <v>0.85961887987408425</v>
       </c>
       <c r="O44" s="1">
-        <f>AI8/AJ8</f>
+        <f t="shared" si="40"/>
         <v>0.83145426790016741</v>
       </c>
       <c r="P44" s="1">
-        <f>AM8/AN8</f>
+        <f t="shared" si="41"/>
         <v>0.80519597917269314</v>
       </c>
       <c r="Q44" s="1">
-        <f>AQ8/AR8</f>
+        <f t="shared" si="42"/>
         <v>0.78907620172518689</v>
       </c>
       <c r="R44" s="1">
-        <f>AU8/AV8</f>
+        <f t="shared" si="43"/>
         <v>0.78479001945421123</v>
       </c>
       <c r="S44" s="1">
-        <f>AY8/AZ8</f>
+        <f t="shared" si="44"/>
         <v>0.78456706403026621</v>
       </c>
       <c r="T44" s="1">
-        <f>BC8/BD8</f>
+        <f t="shared" si="45"/>
         <v>0.78510862385976188</v>
       </c>
     </row>
     <row r="45" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F45" s="1">
+        <f t="shared" si="46"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="G45" s="1">
         <f t="shared" si="32"/>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="G45" s="1">
-        <f>C9/D9</f>
         <v>0.93255003485014432</v>
       </c>
       <c r="H45" s="1">
-        <f>G9/H9</f>
+        <f t="shared" si="33"/>
         <v>0.93088574381808065</v>
       </c>
       <c r="I45" s="1">
-        <f>K9/L9</f>
+        <f t="shared" si="34"/>
         <v>0.92896402563644653</v>
       </c>
       <c r="J45" s="1">
-        <f>O9/P9</f>
+        <f t="shared" si="35"/>
         <v>0.92509777584640296</v>
       </c>
       <c r="K45" s="1">
-        <f>S9/T9</f>
+        <f t="shared" si="36"/>
         <v>0.91635964568472217</v>
       </c>
       <c r="L45" s="1">
-        <f>W9/X9</f>
+        <f t="shared" si="37"/>
         <v>0.90519480519480522</v>
       </c>
       <c r="M45" s="1">
-        <f>AA9/AB9</f>
+        <f t="shared" si="38"/>
         <v>0.88920160827110861</v>
       </c>
       <c r="N45" s="1">
-        <f>AE9/AF9</f>
+        <f t="shared" si="39"/>
         <v>0.86109599834906103</v>
       </c>
       <c r="O45" s="1">
-        <f>AI9/AJ9</f>
+        <f t="shared" si="40"/>
         <v>0.8318401736602955</v>
       </c>
       <c r="P45" s="1">
-        <f>AM9/AN9</f>
+        <f t="shared" si="41"/>
         <v>0.80483704788243582</v>
       </c>
       <c r="Q45" s="1">
-        <f>AQ9/AR9</f>
+        <f t="shared" si="42"/>
         <v>0.78854995974595232</v>
       </c>
       <c r="R45" s="1">
-        <f>AU9/AV9</f>
+        <f t="shared" si="43"/>
         <v>0.78510862385976188</v>
       </c>
       <c r="S45" s="1">
-        <f>AY9/AZ9</f>
+        <f t="shared" si="44"/>
         <v>0.78472631222002109</v>
       </c>
       <c r="T45" s="1">
-        <f>BC9/BD9</f>
+        <f t="shared" si="45"/>
         <v>0.78491744756804993</v>
       </c>
     </row>
     <row r="46" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F46" s="1">
+        <f t="shared" si="46"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="G46" s="1">
         <f t="shared" si="32"/>
-        <v>0.54999999999999993</v>
-      </c>
-      <c r="G46" s="1">
-        <f>C10/D10</f>
         <v>0.93925940873776603</v>
       </c>
       <c r="H46" s="1">
-        <f>G10/H10</f>
+        <f t="shared" si="33"/>
         <v>0.93772148840206182</v>
       </c>
       <c r="I46" s="1">
-        <f>K10/L10</f>
+        <f t="shared" si="34"/>
         <v>0.9360767239822636</v>
       </c>
       <c r="J46" s="1">
-        <f>O10/P10</f>
+        <f t="shared" si="35"/>
         <v>0.93124589446025841</v>
       </c>
       <c r="K46" s="1">
-        <f>S10/T10</f>
+        <f t="shared" si="36"/>
         <v>0.92297526529646146</v>
       </c>
       <c r="L46" s="1">
-        <f>W10/X10</f>
+        <f t="shared" si="37"/>
         <v>0.90863270151403108</v>
       </c>
       <c r="M46" s="1">
-        <f>AA10/AB10</f>
+        <f t="shared" si="38"/>
         <v>0.88952931714603034</v>
       </c>
       <c r="N46" s="1">
-        <f>AE10/AF10</f>
+        <f t="shared" si="39"/>
         <v>0.86079534796473456</v>
       </c>
       <c r="O46" s="1">
-        <f>AI10/AJ10</f>
+        <f t="shared" si="40"/>
         <v>0.83212820371290308</v>
       </c>
       <c r="P46" s="1">
-        <f>AM10/AN10</f>
+        <f t="shared" si="41"/>
         <v>0.80504736423457957</v>
       </c>
       <c r="Q46" s="1">
-        <f>AQ10/AR10</f>
+        <f t="shared" si="42"/>
         <v>0.78853206905805528</v>
       </c>
       <c r="R46" s="1">
-        <f>AU10/AV10</f>
+        <f t="shared" si="43"/>
         <v>0.78529984110831408</v>
       </c>
       <c r="S46" s="1">
-        <f>AY10/AZ10</f>
+        <f t="shared" si="44"/>
         <v>0.78475816526860609</v>
       </c>
       <c r="T46" s="1">
-        <f>BC10/BD10</f>
+        <f t="shared" si="45"/>
         <v>0.78494930743966873</v>
       </c>
     </row>
     <row r="47" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F47" s="1">
+        <f t="shared" si="46"/>
+        <v>0.6</v>
+      </c>
+      <c r="G47" s="1">
         <f t="shared" si="32"/>
-        <v>0.6</v>
-      </c>
-      <c r="G47" s="1">
-        <f>C11/D11</f>
         <v>0.93607333780515067</v>
       </c>
       <c r="H47" s="1">
-        <f>G11/H11</f>
+        <f t="shared" si="33"/>
         <v>0.93493067380199468</v>
       </c>
       <c r="I47" s="1">
-        <f>K11/L11</f>
+        <f t="shared" si="34"/>
         <v>0.93672646643821811</v>
       </c>
       <c r="J47" s="1">
-        <f>O11/P11</f>
+        <f t="shared" si="35"/>
         <v>0.9313899822181374</v>
       </c>
       <c r="K47" s="1">
-        <f>S11/T11</f>
+        <f t="shared" si="36"/>
         <v>0.9230146986287856</v>
       </c>
       <c r="L47" s="1">
-        <f>W11/X11</f>
+        <f t="shared" si="37"/>
         <v>0.90952102803738322</v>
       </c>
       <c r="M47" s="1">
-        <f>AA11/AB11</f>
+        <f t="shared" si="38"/>
         <v>0.88952931714603034</v>
       </c>
       <c r="N47" s="1">
-        <f>AE11/AF11</f>
+        <f t="shared" si="39"/>
         <v>0.86130030959752313</v>
       </c>
       <c r="O47" s="1">
-        <f>AI11/AJ11</f>
+        <f t="shared" si="40"/>
         <v>0.83212820371290308</v>
       </c>
       <c r="P47" s="1">
-        <f>AM11/AN11</f>
+        <f t="shared" si="41"/>
         <v>0.80522861636925747</v>
       </c>
       <c r="Q47" s="1">
-        <f>AQ11/AR11</f>
+        <f t="shared" si="42"/>
         <v>0.78891612833956648</v>
       </c>
       <c r="R47" s="1">
-        <f>AU11/AV11</f>
+        <f t="shared" si="43"/>
         <v>0.78491744756804993</v>
       </c>
       <c r="S47" s="1">
-        <f>AY11/AZ11</f>
+        <f t="shared" si="44"/>
         <v>0.7851723583912027</v>
       </c>
       <c r="T47" s="1">
-        <f>BC11/BD11</f>
+        <f t="shared" si="45"/>
         <v>0.78485373123672508</v>
       </c>
     </row>
     <row r="48" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F48" s="1">
+        <f t="shared" si="46"/>
+        <v>0.65</v>
+      </c>
+      <c r="G48" s="1">
         <f t="shared" si="32"/>
-        <v>0.65</v>
-      </c>
-      <c r="G48" s="1">
-        <f>C12/D12</f>
         <v>0.93241314630565975</v>
       </c>
       <c r="H48" s="1">
-        <f>G12/H12</f>
+        <f t="shared" si="33"/>
         <v>0.93172021146807649</v>
       </c>
       <c r="I48" s="1">
-        <f>K12/L12</f>
+        <f t="shared" si="34"/>
         <v>0.93549299188108415</v>
       </c>
       <c r="J48" s="1">
-        <f>O12/P12</f>
+        <f t="shared" si="35"/>
         <v>0.9317277109879778</v>
       </c>
       <c r="K48" s="1">
-        <f>S12/T12</f>
+        <f t="shared" si="36"/>
         <v>0.92329107925601228</v>
       </c>
       <c r="L48" s="1">
-        <f>W12/X12</f>
+        <f t="shared" si="37"/>
         <v>0.90935461890392277</v>
       </c>
       <c r="M48" s="1">
-        <f>AA12/AB12</f>
+        <f t="shared" si="38"/>
         <v>0.88931224630466421</v>
       </c>
       <c r="N48" s="1">
-        <f>AE12/AF12</f>
+        <f t="shared" si="39"/>
         <v>0.86104232327780283</v>
       </c>
       <c r="O48" s="1">
-        <f>AI12/AJ12</f>
+        <f t="shared" si="40"/>
         <v>0.83214351425942967</v>
       </c>
       <c r="P48" s="1">
-        <f>AM12/AN12</f>
+        <f t="shared" si="41"/>
         <v>0.80509455110821859</v>
       </c>
       <c r="Q48" s="1">
-        <f>AQ12/AR12</f>
+        <f t="shared" si="42"/>
         <v>0.78843608000286236</v>
       </c>
       <c r="R48" s="1">
-        <f>AU12/AV12</f>
+        <f t="shared" si="43"/>
         <v>0.78510862385976188</v>
       </c>
       <c r="S48" s="1">
-        <f>AY12/AZ12</f>
+        <f t="shared" si="44"/>
         <v>0.78479001945421123</v>
       </c>
       <c r="T48" s="1">
-        <f>BC12/BD12</f>
+        <f t="shared" si="45"/>
         <v>0.78466260953366773</v>
       </c>
     </row>
     <row r="49" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F49" s="1">
+        <f t="shared" si="46"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="G49" s="1">
         <f t="shared" si="32"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="G49" s="1">
-        <f>C13/D13</f>
         <v>0.92903963570276282</v>
       </c>
       <c r="H49" s="1">
-        <f>G13/H13</f>
+        <f t="shared" si="33"/>
         <v>0.92821797299773967</v>
       </c>
       <c r="I49" s="1">
-        <f>K13/L13</f>
+        <f t="shared" si="34"/>
         <v>0.93227365568565601</v>
       </c>
       <c r="J49" s="1">
-        <f>O13/P13</f>
+        <f t="shared" si="35"/>
         <v>0.93184500590129826</v>
       </c>
       <c r="K49" s="1">
-        <f>S13/T13</f>
+        <f t="shared" si="36"/>
         <v>0.92321513189069648</v>
       </c>
       <c r="L49" s="1">
-        <f>W13/X13</f>
+        <f t="shared" si="37"/>
         <v>0.90912807335163226</v>
       </c>
       <c r="M49" s="1">
-        <f>AA13/AB13</f>
+        <f t="shared" si="38"/>
         <v>0.88990614824746206</v>
       </c>
       <c r="N49" s="1">
-        <f>AE13/AF13</f>
+        <f t="shared" si="39"/>
         <v>0.86156357904218583</v>
       </c>
       <c r="O49" s="1">
-        <f>AI13/AJ13</f>
+        <f t="shared" si="40"/>
         <v>0.83177277827854523</v>
       </c>
       <c r="P49" s="1">
-        <f>AM13/AN13</f>
+        <f t="shared" si="41"/>
         <v>0.80462325362829623</v>
       </c>
       <c r="Q49" s="1">
-        <f>AQ13/AR13</f>
+        <f t="shared" si="42"/>
         <v>0.78910821984000568</v>
       </c>
       <c r="R49" s="1">
-        <f>AU13/AV13</f>
+        <f t="shared" si="43"/>
         <v>0.78514049055660673</v>
       </c>
       <c r="S49" s="1">
-        <f>AY13/AZ13</f>
+        <f t="shared" si="44"/>
         <v>0.78507675830060697</v>
       </c>
       <c r="T49" s="1">
-        <f>BC13/BD13</f>
+        <f t="shared" si="45"/>
         <v>0.78456706403026621</v>
       </c>
       <c r="U49" s="1" t="s">
@@ -12067,63 +12044,63 @@
     </row>
     <row r="50" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F50" s="1">
+        <f t="shared" si="46"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="G50" s="1">
         <f t="shared" si="32"/>
-        <v>0.75000000000000011</v>
-      </c>
-      <c r="G50" s="1">
-        <f>C14/D14</f>
         <v>0.92851310525026542</v>
       </c>
       <c r="H50" s="1">
-        <f>G14/H14</f>
+        <f t="shared" si="33"/>
         <v>0.9281176183106622</v>
       </c>
       <c r="I50" s="1">
-        <f>K14/L14</f>
+        <f t="shared" si="34"/>
         <v>0.93227639481506941</v>
       </c>
       <c r="J50" s="1">
-        <f>O14/P14</f>
+        <f t="shared" si="35"/>
         <v>0.93180772539057033</v>
       </c>
       <c r="K50" s="1">
-        <f>S14/T14</f>
+        <f t="shared" si="36"/>
         <v>0.92329107925601228</v>
       </c>
       <c r="L50" s="1">
-        <f>W14/X14</f>
+        <f t="shared" si="37"/>
         <v>0.90931744733870656</v>
       </c>
       <c r="M50" s="1">
-        <f>AA14/AB14</f>
+        <f t="shared" si="38"/>
         <v>0.8894037452609812</v>
       </c>
       <c r="N50" s="1">
-        <f>AE14/AF14</f>
+        <f t="shared" si="39"/>
         <v>0.86133783657003471</v>
       </c>
       <c r="O50" s="1">
-        <f>AI14/AJ14</f>
+        <f t="shared" si="40"/>
         <v>0.83189226976709962</v>
       </c>
       <c r="P50" s="1">
-        <f>AM14/AN14</f>
+        <f t="shared" si="41"/>
         <v>0.80464132733286342</v>
       </c>
       <c r="Q50" s="1">
-        <f>AQ14/AR14</f>
+        <f t="shared" si="42"/>
         <v>0.78885210700545771</v>
       </c>
       <c r="R50" s="1">
-        <f>AU14/AV14</f>
+        <f t="shared" si="43"/>
         <v>0.78498116844867283</v>
       </c>
       <c r="S50" s="1">
-        <f>AY14/AZ14</f>
+        <f t="shared" si="44"/>
         <v>0.78475816526860609</v>
       </c>
       <c r="T50" s="1">
-        <f>BC14/BD14</f>
+        <f t="shared" si="45"/>
         <v>0.78472631222002109</v>
       </c>
       <c r="U50" s="1">
@@ -12140,55 +12117,55 @@
         <v>0.87643929513969376</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" ref="H51:T51" si="33">AVERAGE(H37:H50)</f>
+        <f t="shared" ref="H51:T51" si="47">AVERAGE(H37:H50)</f>
         <v>0.87541314889299715</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.87567180168549363</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.87334142192518338</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.86824297809744322</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.8616636980146799</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.85154555035409729</v>
       </c>
       <c r="N51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.83530049525120897</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.81641474119440294</v>
       </c>
       <c r="P51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.79852975582002195</v>
       </c>
       <c r="Q51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.78744094851690394</v>
       </c>
       <c r="R51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.78501304188931509</v>
       </c>
       <c r="S51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.78487422891078762</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="47"/>
         <v>0.78479916076957434</v>
       </c>
       <c r="U51" s="1">

</xml_diff>

<commit_message>
Some testing code for the simple algorithm
</commit_message>
<xml_diff>
--- a/WinningsDistribution.xlsx
+++ b/WinningsDistribution.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="25200" windowHeight="12120" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="25200" windowHeight="12120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alg" sheetId="2" r:id="rId1"/>
-    <sheet name="Complex Alg" sheetId="3" r:id="rId2"/>
-    <sheet name="Complex Alg w Shuffle" sheetId="4" r:id="rId3"/>
-    <sheet name="Complex Alg Comparison" sheetId="5" r:id="rId4"/>
-    <sheet name="Complex w Narrow Range" sheetId="6" r:id="rId5"/>
+    <sheet name="Simple Alg2" sheetId="7" r:id="rId2"/>
+    <sheet name="Complex Alg" sheetId="3" r:id="rId3"/>
+    <sheet name="Complex Alg w Shuffle" sheetId="4" r:id="rId4"/>
+    <sheet name="Complex Alg Comparison" sheetId="5" r:id="rId5"/>
+    <sheet name="Complex w Narrow Range" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -440,11 +441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="280431296"/>
-        <c:axId val="96959968"/>
+        <c:axId val="303611520"/>
+        <c:axId val="303662080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="280431296"/>
+        <c:axId val="303611520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96959968"/>
+        <c:crossAx val="303662080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96959968"/>
+        <c:axId val="303662080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,7 +656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280431296"/>
+        <c:crossAx val="303611520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -910,11 +911,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="96958792"/>
-        <c:axId val="96960360"/>
+        <c:axId val="303664040"/>
+        <c:axId val="303664824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96958792"/>
+        <c:axId val="303664040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96960360"/>
+        <c:crossAx val="303664824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1019,7 +1020,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96960360"/>
+        <c:axId val="303664824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96958792"/>
+        <c:crossAx val="303664040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2982,6 +2983,254 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="C1">
+        <v>6267.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A1+0.25</f>
+        <v>10.25</v>
+      </c>
+      <c r="B2">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="C2">
+        <v>7440.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A33" si="0">A2+0.25</f>
+        <v>10.5</v>
+      </c>
+      <c r="B3">
+        <v>0.67390000000000005</v>
+      </c>
+      <c r="C3">
+        <v>6805.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>10.75</v>
+      </c>
+      <c r="B4">
+        <v>0.6946</v>
+      </c>
+      <c r="C4">
+        <v>7191.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.69550000000000001</v>
+      </c>
+      <c r="C5">
+        <v>7045.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="B6">
+        <v>0.75690000000000002</v>
+      </c>
+      <c r="C6">
+        <v>9276.2999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>14.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>A22+0.25</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>A31+0.25</f>
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD51"/>
   <sheetViews>
     <sheetView topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
@@ -7608,7 +7857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD51"/>
   <sheetViews>
@@ -12223,7 +12472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
@@ -14141,12 +14390,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>